<commit_message>
Continued working on data extraction - working generally.
</commit_message>
<xml_diff>
--- a/resources/db/Case_Data.xlsx
+++ b/resources/db/Case_Data.xlsx
@@ -11,7 +11,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="145621" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -416,18 +416,221 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:B2"/>
+  <dimension ref="A2:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.35"/>
   <sheetData>
     <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>21CRB01291</t>
+        </is>
+      </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>Hemmeter</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>PERMISSION REQ'D TO USE LICENSED DOCK</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1501:46-12-04</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>No Contest</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>19CRB01525</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Pelanda</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>ASSAULT - M1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2903.13(A)</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>M1</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>19CRB01525</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Pelanda</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>AGGRAVATED MENACING</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2903.21</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>M1</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>19CRB01525</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Pelanda</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>DISORDERLY CONDUCT</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2917.11A1</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>MM</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>03TRD13368</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Hemmeter</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>SPEED REDUCED ZONE 3RD OR MORE</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>4511.21C***</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>M3</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Guilty</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>

</xml_diff>